<commit_message>
Add PoisonBubblesParticles.sks. ParticleEngine: update animateParticles so if you put a duration of 0, it doesn't remove the particles from the node at the end of the animation, i.e. animate forever. GameboardSprite: add new PoisonBubblesParticles to marsh tiles upon initializing the game board. Update Levels15MoveList.xlsx
</commit_message>
<xml_diff>
--- a/JSON/Levels15MoveList.xlsx
+++ b/JSON/Levels15MoveList.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B6967647-9F01-544B-8F71-1973D855A32B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099AAA08-553C-DA48-97B5-9E81656A98F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36000" yWindow="-2400" windowWidth="51200" windowHeight="28300"/>
+    <workbookView xWindow="36000" yWindow="-2400" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="csvjson" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19349" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19361" uniqueCount="262">
   <si>
     <t>health</t>
   </si>
@@ -790,11 +790,44 @@
   <si>
     <t>L,R,D,L,U,U,L,U,L,L,D,R,R,U,R,L,U,R,U,L</t>
   </si>
+  <si>
+    <t>D,R,U,R,U,L,R,D</t>
+  </si>
+  <si>
+    <t>D,R,U,L,R,D,L,D,R,R</t>
+  </si>
+  <si>
+    <t>D,R,D,R,U,D</t>
+  </si>
+  <si>
+    <t>D,D,R,D,L,L,U,R</t>
+  </si>
+  <si>
+    <t>D,R,U,D,L,U,R,R,R</t>
+  </si>
+  <si>
+    <t>R,L,D,R,R,R,U,D,D</t>
+  </si>
+  <si>
+    <t>R,R,R,L,L,L,D,D,D,U,R</t>
+  </si>
+  <si>
+    <t>D,R,D,U,R,L,D,R</t>
+  </si>
+  <si>
+    <t>D,U,R,D,R</t>
+  </si>
+  <si>
+    <t>D,D,U,R,D,L,R,U,D,D</t>
+  </si>
+  <si>
+    <t>D,R,R,U,R,D,D</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1727,14 +1760,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CC497"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="2" topLeftCell="K459" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="2" topLeftCell="AE129" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B497" sqref="B497"/>
+      <selection pane="bottomRight" activeCell="B166" sqref="B166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19330,13 +19363,15 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B153" s="8"/>
+      <c r="B153" s="8" t="s">
+        <v>252</v>
+      </c>
       <c r="C153" s="8"/>
       <c r="D153" s="9">
         <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E153" s="9" t="b">
+        <v>10</v>
+      </c>
+      <c r="E153" s="14" t="b">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -19465,15 +19500,17 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B154" s="8"/>
+      <c r="B154" s="8" t="s">
+        <v>253</v>
+      </c>
       <c r="C154" s="8"/>
       <c r="D154" s="9">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E154" s="9" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F154" s="10">
         <f t="shared" si="14"/>
@@ -19590,15 +19627,17 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B155" s="8"/>
+      <c r="B155" s="8" t="s">
+        <v>251</v>
+      </c>
       <c r="C155" s="8"/>
       <c r="D155" s="9">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E155" s="9" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F155" s="10">
         <f t="shared" si="14"/>
@@ -19715,15 +19754,17 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B156" s="8"/>
+      <c r="B156" s="8" t="s">
+        <v>254</v>
+      </c>
       <c r="C156" s="8"/>
       <c r="D156" s="9">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E156" s="9" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F156" s="10">
         <f t="shared" si="14"/>
@@ -19841,15 +19882,17 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B157" s="8"/>
+      <c r="B157" s="8" t="s">
+        <v>255</v>
+      </c>
       <c r="C157" s="8"/>
       <c r="D157" s="9">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E157" s="9" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F157" s="10">
         <f t="shared" si="14"/>
@@ -19967,15 +20010,17 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B158" s="8"/>
+      <c r="B158" s="8" t="s">
+        <v>256</v>
+      </c>
       <c r="C158" s="8"/>
       <c r="D158" s="9">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E158" s="9" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F158" s="10">
         <f t="shared" si="14"/>
@@ -20103,13 +20148,15 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B159" s="8"/>
+      <c r="B159" s="8" t="s">
+        <v>256</v>
+      </c>
       <c r="C159" s="8"/>
       <c r="D159" s="9">
         <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E159" s="9" t="b">
+        <v>9</v>
+      </c>
+      <c r="E159" s="14" t="b">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -20232,15 +20279,17 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B160" s="8"/>
+      <c r="B160" s="8" t="s">
+        <v>257</v>
+      </c>
       <c r="C160" s="8"/>
       <c r="D160" s="9">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E160" s="9" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F160" s="10">
         <f t="shared" si="14"/>
@@ -20367,15 +20416,17 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B161" s="8"/>
+      <c r="B161" s="8" t="s">
+        <v>258</v>
+      </c>
       <c r="C161" s="8"/>
       <c r="D161" s="9">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E161" s="9" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F161" s="10">
         <f t="shared" si="14"/>
@@ -20508,15 +20559,17 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B162" s="8"/>
+      <c r="B162" s="8" t="s">
+        <v>259</v>
+      </c>
       <c r="C162" s="8"/>
       <c r="D162" s="9">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E162" s="9" t="b">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F162" s="10">
         <f t="shared" si="14"/>
@@ -20642,13 +20695,15 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B163" s="8"/>
+      <c r="B163" s="8" t="s">
+        <v>260</v>
+      </c>
       <c r="C163" s="8"/>
       <c r="D163" s="9">
         <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E163" s="9" t="b">
+        <v>10</v>
+      </c>
+      <c r="E163" s="14" t="b">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -20762,13 +20817,15 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B164" s="8"/>
+      <c r="B164" s="8" t="s">
+        <v>138</v>
+      </c>
       <c r="C164" s="8"/>
       <c r="D164" s="9">
         <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E164" s="9" t="b">
+        <v>8</v>
+      </c>
+      <c r="E164" s="14" t="b">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -20893,13 +20950,15 @@
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="B165" s="8"/>
+      <c r="B165" s="8" t="s">
+        <v>261</v>
+      </c>
       <c r="C165" s="8"/>
       <c r="D165" s="9">
         <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E165" s="9" t="b">
+        <v>7</v>
+      </c>
+      <c r="E165" s="14" t="b">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -22065,9 +22124,7 @@
       <c r="BB173" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="BC173" s="13" t="s">
-        <v>84</v>
-      </c>
+      <c r="BC173" s="13"/>
       <c r="BD173" s="13"/>
       <c r="BE173" s="13"/>
       <c r="BF173" t="s">
@@ -83337,7 +83394,7 @@
       <c r="CC497" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:CD497"/>
+  <autoFilter ref="A1:CD497" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Extension+UIFont, et al.: standardize font sizes for gameFont and chatFont with ExtraLarge, Large, Medium and Small. Update all files pertaining...
</commit_message>
<xml_diff>
--- a/JSON/Levels15MoveList.xlsx
+++ b/JSON/Levels15MoveList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099AAA08-553C-DA48-97B5-9E81656A98F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FE6CF0-4B69-B043-A53E-043D3DF3223F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36000" yWindow="-2400" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19361" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19423" uniqueCount="263">
   <si>
     <t>health</t>
   </si>
@@ -822,6 +822,9 @@
   </si>
   <si>
     <t>D,R,R,U,R,D,D</t>
+  </si>
+  <si>
+    <t>R,L,D,D,R,U,L,L,L,D,D,L,D,D,D,R,D,U,L,D,L,R</t>
   </si>
 </sst>
 </file>
@@ -1761,13 +1764,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CC497"/>
+  <dimension ref="A1:CC498"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="2" topLeftCell="AE129" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="2" topLeftCell="K477" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B166" sqref="B166"/>
+      <selection pane="bottomRight" activeCell="B498" sqref="B498"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -73468,7 +73471,7 @@
         <v>0</v>
       </c>
       <c r="F452" s="10">
-        <f t="shared" ref="F452:F497" si="39">F451+1</f>
+        <f t="shared" ref="F452:F498" si="39">F451+1</f>
         <v>450</v>
       </c>
       <c r="G452" s="10">
@@ -83392,6 +83395,226 @@
         <v>87</v>
       </c>
       <c r="CC497" s="13"/>
+    </row>
+    <row r="498" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="A498" s="7">
+        <f t="shared" ref="A498" si="41">COUNTA(J498:O498)</f>
+        <v>6</v>
+      </c>
+      <c r="B498" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="C498" s="8"/>
+      <c r="D498" s="9">
+        <f t="shared" ref="D498" si="42">LEN(B498)-LEN(SUBSTITUTE(B498,",",""))+1</f>
+        <v>22</v>
+      </c>
+      <c r="E498" s="14" t="b">
+        <f t="shared" ref="E498" si="43">D498=H498</f>
+        <v>0</v>
+      </c>
+      <c r="F498" s="10">
+        <f t="shared" si="39"/>
+        <v>496</v>
+      </c>
+      <c r="G498" s="10">
+        <f t="shared" ref="G498" si="44">F498</f>
+        <v>496</v>
+      </c>
+      <c r="H498" s="11">
+        <v>29</v>
+      </c>
+      <c r="I498" s="11">
+        <v>1</v>
+      </c>
+      <c r="J498" t="s">
+        <v>75</v>
+      </c>
+      <c r="K498" t="s">
+        <v>88</v>
+      </c>
+      <c r="L498" t="s">
+        <v>88</v>
+      </c>
+      <c r="M498" t="s">
+        <v>88</v>
+      </c>
+      <c r="N498" t="s">
+        <v>88</v>
+      </c>
+      <c r="O498" t="s">
+        <v>88</v>
+      </c>
+      <c r="P498" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q498" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="R498" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="S498" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="T498" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="U498" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="V498" t="s">
+        <v>88</v>
+      </c>
+      <c r="W498" t="s">
+        <v>88</v>
+      </c>
+      <c r="X498" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y498" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z498" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA498" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB498" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC498" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AD498" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE498" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF498" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG498" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH498" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI498" t="s">
+        <v>89</v>
+      </c>
+      <c r="AJ498" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK498" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL498" t="s">
+        <v>89</v>
+      </c>
+      <c r="AM498" t="s">
+        <v>81</v>
+      </c>
+      <c r="AN498" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AO498" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AP498" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AQ498" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AR498" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AS498" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU498" t="s">
+        <v>78</v>
+      </c>
+      <c r="AV498" t="s">
+        <v>78</v>
+      </c>
+      <c r="AX498" t="s">
+        <v>78</v>
+      </c>
+      <c r="AY498" t="s">
+        <v>78</v>
+      </c>
+      <c r="AZ498" s="13"/>
+      <c r="BA498" s="13"/>
+      <c r="BB498" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BC498" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="BD498" s="13"/>
+      <c r="BE498" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="BF498" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG498" t="s">
+        <v>82</v>
+      </c>
+      <c r="BH498" t="s">
+        <v>78</v>
+      </c>
+      <c r="BI498" t="s">
+        <v>84</v>
+      </c>
+      <c r="BJ498" t="s">
+        <v>83</v>
+      </c>
+      <c r="BK498" t="s">
+        <v>78</v>
+      </c>
+      <c r="BL498" s="13"/>
+      <c r="BM498" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="BN498" s="13"/>
+      <c r="BO498" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BP498" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="BQ498" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BU498" t="s">
+        <v>78</v>
+      </c>
+      <c r="BW498" t="s">
+        <v>87</v>
+      </c>
+      <c r="BX498" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="BY498" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="BZ498" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="CA498" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="CB498" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="CC498" s="13" t="s">
+        <v>83</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:CD497" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Levels15MoveList: add 497 LevelSelectPage: Rename from LevelSelectEngine. Add delegate method didTapLevelSelect(). Inherits from ParentPage. dismissNode is now SettingsTapButton and useMorningSky to get proper coloring. Add touch functions. TitleScene: refactor. Add new closeButtonSprite. Add enum for MenuPage so closeButton knows which page to close. Add Level Selector feature. For now, Start Game button works like Start Game on the Main Menu. Refactor show*() methods - add helper showSecondMenu() template for showLevelSelect and showSettings. CloseButtonSprite: Create this sprite used by TitleScene Main Menu to go back to the Main Menu either from Level Select or Settings pages.
</commit_message>
<xml_diff>
--- a/JSON/Levels15MoveList.xlsx
+++ b/JSON/Levels15MoveList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FE6CF0-4B69-B043-A53E-043D3DF3223F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D52934-0F91-204A-8C48-226CEF4A54FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36000" yWindow="-2400" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="csvjson" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19423" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19489" uniqueCount="264">
   <si>
     <t>health</t>
   </si>
@@ -825,6 +825,9 @@
   </si>
   <si>
     <t>R,L,D,D,R,U,L,L,L,D,D,L,D,D,D,R,D,U,L,D,L,R</t>
+  </si>
+  <si>
+    <t>R,U,R,U,D,D,D,L,L,L,D,L,D,R,R,U,R,R,D,R,D,U,U,R,R,U,L</t>
   </si>
 </sst>
 </file>
@@ -1764,13 +1767,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CC498"/>
+  <dimension ref="A1:CC499"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="10" ySplit="2" topLeftCell="K477" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B498" sqref="B498"/>
+      <selection pane="bottomRight" activeCell="B499" sqref="B499"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -73471,7 +73474,7 @@
         <v>0</v>
       </c>
       <c r="F452" s="10">
-        <f t="shared" ref="F452:F498" si="39">F451+1</f>
+        <f t="shared" ref="F452:F499" si="39">F451+1</f>
         <v>450</v>
       </c>
       <c r="G452" s="10">
@@ -83614,6 +83617,236 @@
       </c>
       <c r="CC498" s="13" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="499" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="A499" s="7">
+        <f t="shared" ref="A499" si="45">COUNTA(J499:O499)</f>
+        <v>6</v>
+      </c>
+      <c r="B499" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="C499" s="8"/>
+      <c r="D499" s="9">
+        <f t="shared" ref="D499" si="46">LEN(B499)-LEN(SUBSTITUTE(B499,",",""))+1</f>
+        <v>27</v>
+      </c>
+      <c r="E499" s="14" t="b">
+        <f t="shared" ref="E499" si="47">D499=H499</f>
+        <v>0</v>
+      </c>
+      <c r="F499" s="10">
+        <f t="shared" si="39"/>
+        <v>497</v>
+      </c>
+      <c r="G499" s="10">
+        <f t="shared" ref="G499" si="48">F499</f>
+        <v>497</v>
+      </c>
+      <c r="H499" s="11">
+        <v>29</v>
+      </c>
+      <c r="I499" s="11">
+        <v>1</v>
+      </c>
+      <c r="J499" t="s">
+        <v>77</v>
+      </c>
+      <c r="K499" t="s">
+        <v>85</v>
+      </c>
+      <c r="L499" t="s">
+        <v>85</v>
+      </c>
+      <c r="M499" t="s">
+        <v>89</v>
+      </c>
+      <c r="N499" t="s">
+        <v>85</v>
+      </c>
+      <c r="O499" t="s">
+        <v>88</v>
+      </c>
+      <c r="P499" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q499" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="R499" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="S499" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="T499" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="U499" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="V499" t="s">
+        <v>88</v>
+      </c>
+      <c r="W499" t="s">
+        <v>89</v>
+      </c>
+      <c r="X499" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y499" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z499" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA499" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB499" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC499" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD499" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE499" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF499" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG499" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH499" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI499" t="s">
+        <v>88</v>
+      </c>
+      <c r="AJ499" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK499" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL499" t="s">
+        <v>88</v>
+      </c>
+      <c r="AM499" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN499" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO499" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AP499" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AQ499" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="AR499" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AS499" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AT499" t="s">
+        <v>83</v>
+      </c>
+      <c r="AU499" t="s">
+        <v>78</v>
+      </c>
+      <c r="AX499" t="s">
+        <v>78</v>
+      </c>
+      <c r="AY499" t="s">
+        <v>90</v>
+      </c>
+      <c r="AZ499" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="BA499" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BB499" s="13"/>
+      <c r="BC499" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="BD499" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="BE499" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BF499" t="s">
+        <v>78</v>
+      </c>
+      <c r="BI499" t="s">
+        <v>80</v>
+      </c>
+      <c r="BJ499" t="s">
+        <v>80</v>
+      </c>
+      <c r="BK499" t="s">
+        <v>78</v>
+      </c>
+      <c r="BL499" s="13"/>
+      <c r="BM499" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="BN499" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BO499" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="BP499" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="BQ499" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="BR499" t="s">
+        <v>79</v>
+      </c>
+      <c r="BS499" t="s">
+        <v>79</v>
+      </c>
+      <c r="BT499" t="s">
+        <v>79</v>
+      </c>
+      <c r="BU499" t="s">
+        <v>78</v>
+      </c>
+      <c r="BV499" t="s">
+        <v>90</v>
+      </c>
+      <c r="BW499" t="s">
+        <v>87</v>
+      </c>
+      <c r="BX499" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="BY499" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="BZ499" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="CA499" s="13"/>
+      <c r="CB499" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="CC499" s="13" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>